<commit_message>
Convertit, écrit la note/20 dans un emplacement libre de la colonne Français - Mettre la note moyenne de sur la ligne 20 - Laisser l'user choisir la colonne utilisé - ...
</commit_message>
<xml_diff>
--- a/Note.xlsx
+++ b/Note.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -472,46 +472,14 @@
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
     <row r="20">
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="n"/>

</xml_diff>

<commit_message>
- Demande la colonne besoin - Fait la moyenne en bas de la colonne - Demande plusieurs fois les notes - À FAIRE, colonne acquis / non acquis   + couleur si + 50%
</commit_message>
<xml_diff>
--- a/Note.xlsx
+++ b/Note.xlsx
@@ -1,33 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\SoloBolo\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F2C2C1-1001-4757-A197-09CAB6E467A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2445" yWindow="1515" windowWidth="20910" windowHeight="11835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2595" yWindow="210" windowWidth="24090" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Note_cour" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Note_cour" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Architecture d'ordinateur</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Programmation</t>
+  </si>
+  <si>
+    <t>Système d'exploitation</t>
+  </si>
+  <si>
+    <t>Gestion de base de données</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Acquis/Non acquis</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,82 +77,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,84 +393,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G220" sqref="G220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="24.42578125" customWidth="1" style="1" min="1" max="1"/>
-    <col width="8.7109375" customWidth="1" style="1" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="22.28515625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="27" customWidth="1" style="1" min="5" max="5"/>
-    <col width="9.28515625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="17.85546875" customWidth="1" style="1" min="7" max="7"/>
+    <col min="1" max="1" width="24.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Architecture d'ordinateur</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Français</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Programmation</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Système d'exploitation</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Gestion de base de données</t>
-        </is>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="n">
-        <v>14</v>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="20">
-      <c r="A20" s="2" t="n"/>
-      <c r="B20" s="2" t="n"/>
-      <c r="C20" s="2" t="n"/>
-      <c r="D20" s="2" t="n"/>
-      <c r="E20" s="2" t="n"/>
-      <c r="F20" s="2" t="n"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="21">
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Acquis/Non acquis</t>
-        </is>
-      </c>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220"/>
+      <c r="B220"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>